<commit_message>
SQL DATABASE AUTOMATION TESTING
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/HRMSdata.xlsx
+++ b/src/test/resources/Excel/HRMSdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beyha\eclipse-workspace\HRMSCucumber\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9988A187-E6FC-4078-BFE4-7640AD741EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7F5BB2-60DE-4300-AC9B-6A2D23811876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>firstName</t>
   </si>
@@ -109,18 +109,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>Ann</t>
-  </si>
-  <si>
-    <t>mary56234234345345</t>
-  </si>
-  <si>
-    <t>Tarlaci</t>
-  </si>
-  <si>
-    <t>ali562342342353</t>
-  </si>
-  <si>
     <t>john58694535</t>
   </si>
   <si>
@@ -130,22 +118,40 @@
     <t>Jack</t>
   </si>
   <si>
-    <t>Mimi</t>
-  </si>
-  <si>
-    <t>Veli</t>
-  </si>
-  <si>
-    <t>AmirKhan_*@123</t>
-  </si>
-  <si>
     <t>Johnn</t>
   </si>
   <si>
-    <t>Maryy</t>
-  </si>
-  <si>
-    <t>Alii</t>
+    <t>Haryy</t>
+  </si>
+  <si>
+    <t>Mimis</t>
+  </si>
+  <si>
+    <t>Annys</t>
+  </si>
+  <si>
+    <t>mary567298045</t>
+  </si>
+  <si>
+    <t>Jordon</t>
+  </si>
+  <si>
+    <t>Jelli</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Jor35323765</t>
+  </si>
+  <si>
+    <t>JohKhan_*@123</t>
+  </si>
+  <si>
+    <t>mayrKhan_*@123</t>
+  </si>
+  <si>
+    <t>jorKhan_*@123</t>
   </si>
 </sst>
 </file>
@@ -611,7 +617,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +634,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>23</v>
@@ -643,55 +649,55 @@
     </row>
     <row r="2" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F4" s="2"/>
     </row>

</xml_diff>